<commit_message>
Add new joinee to database, sep dependant async fn
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="572">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -1688,6 +1688,54 @@
   </si>
   <si>
     <t xml:space="preserve">21F2000219</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21F1000164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21F1000925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21F1001180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21F1001914</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21F1002604</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21F1002644</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21F1003008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21F1003057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21F1003406</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21F1003511</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21F1004030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21F1004033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21F1004833</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21F1005277</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21F1005925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21F2000104</t>
   </si>
 </sst>
 </file>
@@ -1784,16 +1832,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B555"/>
+  <dimension ref="A1:B571"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:A555"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:A571"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6234,6 +6282,134 @@
       </c>
       <c r="B555" s="0" t="n">
         <v>52</v>
+      </c>
+    </row>
+    <row r="556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A556" s="0" t="s">
+        <v>556</v>
+      </c>
+      <c r="B556" s="0" t="n">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A557" s="0" t="s">
+        <v>557</v>
+      </c>
+      <c r="B557" s="0" t="n">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A558" s="0" t="s">
+        <v>558</v>
+      </c>
+      <c r="B558" s="0" t="n">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A559" s="0" t="s">
+        <v>559</v>
+      </c>
+      <c r="B559" s="0" t="n">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A560" s="0" t="s">
+        <v>560</v>
+      </c>
+      <c r="B560" s="0" t="n">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A561" s="0" t="s">
+        <v>561</v>
+      </c>
+      <c r="B561" s="0" t="n">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A562" s="0" t="s">
+        <v>562</v>
+      </c>
+      <c r="B562" s="0" t="n">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A563" s="0" t="s">
+        <v>563</v>
+      </c>
+      <c r="B563" s="0" t="n">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A564" s="0" t="s">
+        <v>564</v>
+      </c>
+      <c r="B564" s="0" t="n">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A565" s="0" t="s">
+        <v>565</v>
+      </c>
+      <c r="B565" s="0" t="n">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A566" s="0" t="s">
+        <v>566</v>
+      </c>
+      <c r="B566" s="0" t="n">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A567" s="0" t="s">
+        <v>567</v>
+      </c>
+      <c r="B567" s="0" t="n">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A568" s="0" t="s">
+        <v>568</v>
+      </c>
+      <c r="B568" s="0" t="n">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A569" s="0" t="s">
+        <v>569</v>
+      </c>
+      <c r="B569" s="0" t="n">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A570" s="0" t="s">
+        <v>570</v>
+      </c>
+      <c r="B570" s="0" t="n">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A571" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="B571" s="0" t="n">
+        <v>311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>